<commit_message>
Fix typo in Excel first sheet.
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -112,9 +112,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="73">
-  <si>
-    <t>Заказа наряд №</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
+  <si>
+    <t>Заказ наряд №</t>
   </si>
   <si>
     <t>Заказчик</t>
@@ -159,7 +159,7 @@
     <t>Дата выполнения</t>
   </si>
   <si>
-    <t>Форма раслета</t>
+    <t>Форма расчета</t>
   </si>
   <si>
     <t>Форма доставки</t>
@@ -223,12 +223,6 @@
   </si>
   <si>
     <t>отказ от доставки</t>
-  </si>
-  <si>
-    <t>Заказ наряд №</t>
-  </si>
-  <si>
-    <t>Форма расчета</t>
   </si>
   <si>
     <t>Примечание</t>
@@ -1143,7 +1137,7 @@
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="L1" activeCellId="0" pane="bottomLeft" sqref="L1"/>
+      <selection activeCell="Q3" activeCellId="0" pane="bottomLeft" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1387,7 +1381,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="9"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
       <c r="B10" s="27" t="s">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
@@ -1470,7 +1464,7 @@
       <c r="O12" s="33"/>
       <c r="P12" s="33"/>
       <c r="R12" s="29" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="S12" s="29"/>
       <c r="T12" s="29"/>
@@ -1633,7 +1627,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="7.5" outlineLevel="0" r="18"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
@@ -1774,7 +1768,7 @@
       <c r="A24" s="42"/>
       <c r="B24" s="42"/>
       <c r="C24" s="43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
@@ -1782,7 +1776,7 @@
       <c r="G24" s="43"/>
       <c r="H24" s="43"/>
       <c r="I24" s="44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J24" s="44"/>
       <c r="K24" s="44"/>
@@ -1796,19 +1790,19 @@
       <c r="S24" s="44"/>
       <c r="T24" s="44"/>
       <c r="U24" s="45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="V24" s="45"/>
       <c r="W24" s="45"/>
       <c r="X24" s="46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="Y24" s="46"/>
       <c r="Z24" s="46"/>
       <c r="AA24" s="46"/>
       <c r="AB24" s="46"/>
       <c r="AC24" s="47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AD24" s="47"/>
       <c r="AE24" s="47"/>
@@ -2407,7 +2401,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="41">
       <c r="Q41" s="64" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R41" s="64"/>
       <c r="S41" s="64"/>
@@ -2463,7 +2457,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" s="29"/>
       <c r="C43" s="29"/>
@@ -2535,7 +2529,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="20.25" outlineLevel="0" r="45">
       <c r="S45" s="35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="T45" s="35"/>
       <c r="U45" s="35"/>
@@ -2560,7 +2554,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9" outlineLevel="0" r="46">
       <c r="X46" s="68"/>
       <c r="Y46" s="69" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Z46" s="69"/>
       <c r="AA46" s="69"/>
@@ -2612,7 +2606,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.75" outlineLevel="0" r="48">
       <c r="A48" s="71" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B48" s="71"/>
       <c r="C48" s="71"/>
@@ -2719,7 +2713,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51">
       <c r="A51" s="72" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B51" s="72"/>
       <c r="C51" s="72"/>
@@ -2757,7 +2751,7 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.5" outlineLevel="0" r="52"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
       <c r="A53" s="73" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B53" s="73"/>
       <c r="C53" s="73"/>
@@ -2773,7 +2767,7 @@
       <c r="M53" s="73"/>
       <c r="N53" s="73"/>
       <c r="S53" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T53" s="27"/>
       <c r="U53" s="27"/>
@@ -2823,7 +2817,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="8.25" outlineLevel="0" r="55">
       <c r="A55" s="74" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B55" s="74"/>
       <c r="C55" s="74"/>
@@ -2840,7 +2834,7 @@
       <c r="N55" s="74"/>
       <c r="R55" s="68"/>
       <c r="S55" s="74" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="T55" s="74"/>
       <c r="U55" s="74"/>
@@ -3039,25 +3033,25 @@
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="1" s="10">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="75" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="75" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="75" t="s">
+      <c r="G1" s="75" t="s">
         <v>55</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="75" t="s">
-        <v>57</v>
       </c>
       <c r="H1" s="75"/>
       <c r="I1" s="75"/>
@@ -3074,10 +3068,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="76" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="66" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C2" s="77"/>
       <c r="D2" s="77"/>
@@ -3101,10 +3095,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="76" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" s="77"/>
       <c r="D3" s="77"/>
@@ -3118,10 +3112,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="76" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B4" s="66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="77"/>
       <c r="D4" s="77"/>
@@ -3165,15 +3159,15 @@
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="1">
       <c r="A1" s="79" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="79" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
       <c r="A2" s="80" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B2" s="81" t="n">
         <v>0.05</v>
@@ -3181,7 +3175,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
       <c r="A3" s="80" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="81" t="n">
         <v>0.07</v>
@@ -3189,7 +3183,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
       <c r="A4" s="80" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B4" s="81" t="n">
         <v>0.1</v>
@@ -3197,7 +3191,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
       <c r="A5" s="80" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="81" t="n">
         <v>0.12</v>
@@ -3205,7 +3199,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
       <c r="A6" s="80" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B6" s="81" t="n">
         <v>0.15</v>
@@ -3213,10 +3207,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
       <c r="A7" s="80" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve label with symbol D, add save for column width, table products, remove currency symbol. github: #15
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -237,7 +237,7 @@
     <t>Кол-во</t>
   </si>
   <si>
-    <t>Цена                руб.</t>
+    <t>Цена руб.</t>
   </si>
   <si>
     <t>Стоимость руб.</t>
@@ -678,7 +678,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -861,14 +861,6 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1134,9 +1126,9 @@
   </sheetPr>
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="K1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" xSplit="0" ySplit="1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="K1" activeCellId="0" pane="topLeft" sqref="K1"/>
       <selection activeCell="Q3" activeCellId="0" pane="bottomLeft" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -1364,7 +1356,7 @@
   <dimension ref="A9:AQ55"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="U41" activeCellId="0" pane="topLeft" sqref="U41"/>
+      <selection activeCell="AC24" activeCellId="0" pane="topLeft" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1794,20 +1786,20 @@
       </c>
       <c r="V24" s="45"/>
       <c r="W24" s="45"/>
-      <c r="X24" s="46" t="s">
+      <c r="X24" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="Y24" s="46"/>
-      <c r="Z24" s="46"/>
-      <c r="AA24" s="46"/>
-      <c r="AB24" s="46"/>
-      <c r="AC24" s="47" t="s">
+      <c r="Y24" s="45"/>
+      <c r="Z24" s="45"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="45"/>
+      <c r="AC24" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="AD24" s="47"/>
-      <c r="AE24" s="47"/>
-      <c r="AF24" s="47"/>
-      <c r="AG24" s="47"/>
+      <c r="AD24" s="44"/>
+      <c r="AE24" s="44"/>
+      <c r="AF24" s="44"/>
+      <c r="AG24" s="44"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="25">
       <c r="A25" s="42"/>
@@ -1833,77 +1825,77 @@
       <c r="U25" s="45"/>
       <c r="V25" s="45"/>
       <c r="W25" s="45"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="46"/>
-      <c r="Z25" s="46"/>
-      <c r="AA25" s="46"/>
-      <c r="AB25" s="46"/>
-      <c r="AC25" s="47"/>
-      <c r="AD25" s="47"/>
-      <c r="AE25" s="47"/>
-      <c r="AF25" s="47"/>
-      <c r="AG25" s="47"/>
+      <c r="X25" s="45"/>
+      <c r="Y25" s="45"/>
+      <c r="Z25" s="45"/>
+      <c r="AA25" s="45"/>
+      <c r="AB25" s="45"/>
+      <c r="AC25" s="44"/>
+      <c r="AD25" s="44"/>
+      <c r="AE25" s="44"/>
+      <c r="AF25" s="44"/>
+      <c r="AG25" s="44"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="26">
-      <c r="A26" s="48" t="n">
+      <c r="A26" s="46" t="n">
         <v>1</v>
       </c>
-      <c r="B26" s="48"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="49"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="53"/>
-      <c r="V26" s="53"/>
-      <c r="W26" s="53"/>
-      <c r="X26" s="54"/>
-      <c r="Y26" s="54"/>
-      <c r="Z26" s="54"/>
-      <c r="AA26" s="54"/>
-      <c r="AB26" s="54"/>
-      <c r="AC26" s="54"/>
-      <c r="AD26" s="54"/>
-      <c r="AE26" s="54"/>
-      <c r="AF26" s="54"/>
-      <c r="AG26" s="54"/>
+      <c r="B26" s="46"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="49"/>
+      <c r="P26" s="49"/>
+      <c r="Q26" s="49"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="51"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="52"/>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="52"/>
+      <c r="AA26" s="52"/>
+      <c r="AB26" s="52"/>
+      <c r="AC26" s="52"/>
+      <c r="AD26" s="52"/>
+      <c r="AE26" s="52"/>
+      <c r="AF26" s="52"/>
+      <c r="AG26" s="52"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="27">
-      <c r="A27" s="55" t="n">
+      <c r="A27" s="53" t="n">
         <v>2</v>
       </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="56"/>
-      <c r="H27" s="56"/>
-      <c r="I27" s="57"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="58"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="59"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54"/>
+      <c r="I27" s="55"/>
+      <c r="J27" s="56"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="56"/>
+      <c r="M27" s="56"/>
+      <c r="N27" s="56"/>
+      <c r="O27" s="56"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="56"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="57"/>
       <c r="U27" s="41"/>
       <c r="V27" s="41"/>
       <c r="W27" s="41"/>
@@ -1919,28 +1911,28 @@
       <c r="AG27" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="28">
-      <c r="A28" s="55" t="n">
+      <c r="A28" s="53" t="n">
         <v>3</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="57"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="58"/>
-      <c r="L28" s="58"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="58"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="59"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="55"/>
+      <c r="J28" s="56"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="56"/>
+      <c r="M28" s="56"/>
+      <c r="N28" s="56"/>
+      <c r="O28" s="56"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="57"/>
       <c r="U28" s="41"/>
       <c r="V28" s="41"/>
       <c r="W28" s="41"/>
@@ -1956,10 +1948,10 @@
       <c r="AG28" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="55" t="n">
+      <c r="A29" s="53" t="n">
         <v>4</v>
       </c>
-      <c r="B29" s="55"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="32"/>
       <c r="D29" s="32"/>
       <c r="E29" s="32"/>
@@ -1993,10 +1985,10 @@
       <c r="AG29" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="A30" s="55" t="n">
+      <c r="A30" s="53" t="n">
         <v>5</v>
       </c>
-      <c r="B30" s="55"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="32"/>
@@ -2030,10 +2022,10 @@
       <c r="AG30" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="A31" s="55" t="n">
+      <c r="A31" s="53" t="n">
         <v>6</v>
       </c>
-      <c r="B31" s="55"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="32"/>
@@ -2067,10 +2059,10 @@
       <c r="AG31" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="A32" s="55" t="n">
+      <c r="A32" s="53" t="n">
         <v>7</v>
       </c>
-      <c r="B32" s="55"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
@@ -2104,10 +2096,10 @@
       <c r="AG32" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="A33" s="55" t="n">
+      <c r="A33" s="53" t="n">
         <v>8</v>
       </c>
-      <c r="B33" s="55"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
@@ -2141,10 +2133,10 @@
       <c r="AG33" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="A34" s="55" t="n">
+      <c r="A34" s="53" t="n">
         <v>9</v>
       </c>
-      <c r="B34" s="55"/>
+      <c r="B34" s="53"/>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
       <c r="E34" s="32"/>
@@ -2178,10 +2170,10 @@
       <c r="AG34" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="A35" s="55" t="n">
+      <c r="A35" s="53" t="n">
         <v>10</v>
       </c>
-      <c r="B35" s="55"/>
+      <c r="B35" s="53"/>
       <c r="C35" s="32"/>
       <c r="D35" s="32"/>
       <c r="E35" s="32"/>
@@ -2215,10 +2207,10 @@
       <c r="AG35" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="A36" s="55" t="n">
+      <c r="A36" s="53" t="n">
         <v>11</v>
       </c>
-      <c r="B36" s="55"/>
+      <c r="B36" s="53"/>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
       <c r="E36" s="32"/>
@@ -2252,10 +2244,10 @@
       <c r="AG36" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="A37" s="55" t="n">
+      <c r="A37" s="53" t="n">
         <v>12</v>
       </c>
-      <c r="B37" s="55"/>
+      <c r="B37" s="53"/>
       <c r="C37" s="32"/>
       <c r="D37" s="32"/>
       <c r="E37" s="32"/>
@@ -2289,10 +2281,10 @@
       <c r="AG37" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="A38" s="55" t="n">
+      <c r="A38" s="53" t="n">
         <v>13</v>
       </c>
-      <c r="B38" s="55"/>
+      <c r="B38" s="53"/>
       <c r="C38" s="32"/>
       <c r="D38" s="32"/>
       <c r="E38" s="32"/>
@@ -2326,10 +2318,10 @@
       <c r="AG38" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="A39" s="55" t="n">
+      <c r="A39" s="53" t="n">
         <v>14</v>
       </c>
-      <c r="B39" s="55"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
       <c r="E39" s="32"/>
@@ -2363,97 +2355,97 @@
       <c r="AG39" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.75" outlineLevel="0" r="40">
-      <c r="A40" s="60" t="n">
+      <c r="A40" s="58" t="n">
         <v>15</v>
       </c>
-      <c r="B40" s="60"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="61"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="61"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="61"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="62"/>
-      <c r="K40" s="62"/>
-      <c r="L40" s="62"/>
-      <c r="M40" s="62"/>
-      <c r="N40" s="62"/>
-      <c r="O40" s="62"/>
-      <c r="P40" s="62"/>
-      <c r="Q40" s="62"/>
-      <c r="R40" s="62"/>
-      <c r="S40" s="62"/>
-      <c r="T40" s="62"/>
-      <c r="U40" s="63"/>
-      <c r="V40" s="63"/>
-      <c r="W40" s="63"/>
-      <c r="X40" s="62"/>
-      <c r="Y40" s="62"/>
-      <c r="Z40" s="62"/>
-      <c r="AA40" s="62"/>
-      <c r="AB40" s="62"/>
-      <c r="AC40" s="62"/>
-      <c r="AD40" s="62"/>
-      <c r="AE40" s="62"/>
-      <c r="AF40" s="62"/>
-      <c r="AG40" s="62"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="59"/>
+      <c r="E40" s="59"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="59"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="60"/>
+      <c r="K40" s="60"/>
+      <c r="L40" s="60"/>
+      <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
+      <c r="P40" s="60"/>
+      <c r="Q40" s="60"/>
+      <c r="R40" s="60"/>
+      <c r="S40" s="60"/>
+      <c r="T40" s="60"/>
+      <c r="U40" s="61"/>
+      <c r="V40" s="61"/>
+      <c r="W40" s="61"/>
+      <c r="X40" s="60"/>
+      <c r="Y40" s="60"/>
+      <c r="Z40" s="60"/>
+      <c r="AA40" s="60"/>
+      <c r="AB40" s="60"/>
+      <c r="AC40" s="60"/>
+      <c r="AD40" s="60"/>
+      <c r="AE40" s="60"/>
+      <c r="AF40" s="60"/>
+      <c r="AG40" s="60"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.5" outlineLevel="0" r="41">
-      <c r="Q41" s="64" t="s">
+      <c r="Q41" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="R41" s="64"/>
-      <c r="S41" s="64"/>
-      <c r="T41" s="64"/>
-      <c r="U41" s="61"/>
-      <c r="V41" s="61"/>
-      <c r="W41" s="61"/>
-      <c r="X41" s="61"/>
-      <c r="Y41" s="61"/>
-      <c r="Z41" s="61"/>
-      <c r="AA41" s="61"/>
-      <c r="AB41" s="61"/>
-      <c r="AC41" s="65"/>
-      <c r="AD41" s="65"/>
-      <c r="AE41" s="65"/>
-      <c r="AF41" s="65"/>
-      <c r="AG41" s="65"/>
+      <c r="R41" s="62"/>
+      <c r="S41" s="62"/>
+      <c r="T41" s="62"/>
+      <c r="U41" s="59"/>
+      <c r="V41" s="59"/>
+      <c r="W41" s="59"/>
+      <c r="X41" s="59"/>
+      <c r="Y41" s="59"/>
+      <c r="Z41" s="59"/>
+      <c r="AA41" s="59"/>
+      <c r="AB41" s="59"/>
+      <c r="AC41" s="63"/>
+      <c r="AD41" s="63"/>
+      <c r="AE41" s="63"/>
+      <c r="AF41" s="63"/>
+      <c r="AG41" s="63"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="A42" s="66"/>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="66"/>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="66"/>
-      <c r="I42" s="66"/>
-      <c r="J42" s="66"/>
-      <c r="K42" s="66"/>
-      <c r="L42" s="66"/>
-      <c r="M42" s="66"/>
-      <c r="N42" s="66"/>
-      <c r="O42" s="66"/>
-      <c r="P42" s="66"/>
-      <c r="Q42" s="66"/>
-      <c r="R42" s="66"/>
-      <c r="S42" s="66"/>
-      <c r="T42" s="66"/>
-      <c r="U42" s="66"/>
-      <c r="V42" s="66"/>
-      <c r="W42" s="66"/>
-      <c r="X42" s="66"/>
-      <c r="Y42" s="66"/>
-      <c r="Z42" s="66"/>
-      <c r="AA42" s="67"/>
-      <c r="AB42" s="67"/>
-      <c r="AC42" s="66"/>
-      <c r="AD42" s="66"/>
-      <c r="AE42" s="66"/>
-      <c r="AF42" s="66"/>
-      <c r="AG42" s="66"/>
+      <c r="A42" s="64"/>
+      <c r="B42" s="64"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="64"/>
+      <c r="N42" s="64"/>
+      <c r="O42" s="64"/>
+      <c r="P42" s="64"/>
+      <c r="Q42" s="64"/>
+      <c r="R42" s="64"/>
+      <c r="S42" s="64"/>
+      <c r="T42" s="64"/>
+      <c r="U42" s="64"/>
+      <c r="V42" s="64"/>
+      <c r="W42" s="64"/>
+      <c r="X42" s="64"/>
+      <c r="Y42" s="64"/>
+      <c r="Z42" s="64"/>
+      <c r="AA42" s="65"/>
+      <c r="AB42" s="65"/>
+      <c r="AC42" s="64"/>
+      <c r="AD42" s="64"/>
+      <c r="AE42" s="64"/>
+      <c r="AF42" s="64"/>
+      <c r="AG42" s="64"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="43">
       <c r="A43" s="29" t="s">
@@ -2545,227 +2537,227 @@
       <c r="AE45" s="40"/>
       <c r="AF45" s="40"/>
       <c r="AG45" s="40"/>
-      <c r="AH45" s="66"/>
-      <c r="AI45" s="66"/>
-      <c r="AJ45" s="66"/>
-      <c r="AK45" s="66"/>
-      <c r="AL45" s="66"/>
+      <c r="AH45" s="64"/>
+      <c r="AI45" s="64"/>
+      <c r="AJ45" s="64"/>
+      <c r="AK45" s="64"/>
+      <c r="AL45" s="64"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="9" outlineLevel="0" r="46">
-      <c r="X46" s="68"/>
-      <c r="Y46" s="69" t="s">
+      <c r="X46" s="66"/>
+      <c r="Y46" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="Z46" s="69"/>
-      <c r="AA46" s="69"/>
-      <c r="AB46" s="69"/>
-      <c r="AC46" s="69"/>
-      <c r="AD46" s="69"/>
-      <c r="AE46" s="69"/>
-      <c r="AF46" s="69"/>
-      <c r="AG46" s="69"/>
-      <c r="AH46" s="68"/>
-      <c r="AI46" s="68"/>
-      <c r="AJ46" s="68"/>
-      <c r="AK46" s="68"/>
+      <c r="Z46" s="67"/>
+      <c r="AA46" s="67"/>
+      <c r="AB46" s="67"/>
+      <c r="AC46" s="67"/>
+      <c r="AD46" s="67"/>
+      <c r="AE46" s="67"/>
+      <c r="AF46" s="67"/>
+      <c r="AG46" s="67"/>
+      <c r="AH46" s="66"/>
+      <c r="AI46" s="66"/>
+      <c r="AJ46" s="66"/>
+      <c r="AK46" s="66"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="5.25" outlineLevel="0" r="47">
-      <c r="B47" s="70"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="70"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="70"/>
-      <c r="N47" s="70"/>
-      <c r="O47" s="70"/>
-      <c r="P47" s="70"/>
-      <c r="Q47" s="70"/>
-      <c r="R47" s="70"/>
-      <c r="S47" s="70"/>
-      <c r="T47" s="70"/>
-      <c r="U47" s="70"/>
-      <c r="V47" s="70"/>
-      <c r="W47" s="70"/>
-      <c r="X47" s="70"/>
-      <c r="Y47" s="70"/>
-      <c r="Z47" s="70"/>
-      <c r="AA47" s="70"/>
-      <c r="AB47" s="70"/>
-      <c r="AC47" s="70"/>
-      <c r="AD47" s="70"/>
-      <c r="AE47" s="70"/>
-      <c r="AF47" s="70"/>
-      <c r="AG47" s="70"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="68"/>
+      <c r="I47" s="68"/>
+      <c r="J47" s="68"/>
+      <c r="K47" s="68"/>
+      <c r="L47" s="68"/>
+      <c r="M47" s="68"/>
+      <c r="N47" s="68"/>
+      <c r="O47" s="68"/>
+      <c r="P47" s="68"/>
+      <c r="Q47" s="68"/>
+      <c r="R47" s="68"/>
+      <c r="S47" s="68"/>
+      <c r="T47" s="68"/>
+      <c r="U47" s="68"/>
+      <c r="V47" s="68"/>
+      <c r="W47" s="68"/>
+      <c r="X47" s="68"/>
+      <c r="Y47" s="68"/>
+      <c r="Z47" s="68"/>
+      <c r="AA47" s="68"/>
+      <c r="AB47" s="68"/>
+      <c r="AC47" s="68"/>
+      <c r="AD47" s="68"/>
+      <c r="AE47" s="68"/>
+      <c r="AF47" s="68"/>
+      <c r="AG47" s="68"/>
       <c r="AQ47" s="5"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="18.75" outlineLevel="0" r="48">
-      <c r="A48" s="71" t="s">
+      <c r="A48" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="71"/>
-      <c r="C48" s="71"/>
-      <c r="D48" s="71"/>
-      <c r="E48" s="71"/>
-      <c r="F48" s="71"/>
-      <c r="G48" s="71"/>
-      <c r="H48" s="71"/>
-      <c r="I48" s="71"/>
-      <c r="J48" s="71"/>
-      <c r="K48" s="71"/>
-      <c r="L48" s="71"/>
-      <c r="M48" s="71"/>
-      <c r="N48" s="71"/>
-      <c r="O48" s="71"/>
-      <c r="P48" s="71"/>
-      <c r="Q48" s="71"/>
-      <c r="R48" s="71"/>
-      <c r="S48" s="71"/>
-      <c r="T48" s="71"/>
-      <c r="U48" s="71"/>
-      <c r="V48" s="71"/>
-      <c r="W48" s="71"/>
-      <c r="X48" s="71"/>
-      <c r="Y48" s="71"/>
-      <c r="Z48" s="71"/>
-      <c r="AA48" s="71"/>
-      <c r="AB48" s="71"/>
-      <c r="AC48" s="71"/>
-      <c r="AD48" s="71"/>
-      <c r="AE48" s="71"/>
-      <c r="AF48" s="71"/>
-      <c r="AG48" s="71"/>
+      <c r="B48" s="69"/>
+      <c r="C48" s="69"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
+      <c r="F48" s="69"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="69"/>
+      <c r="I48" s="69"/>
+      <c r="J48" s="69"/>
+      <c r="K48" s="69"/>
+      <c r="L48" s="69"/>
+      <c r="M48" s="69"/>
+      <c r="N48" s="69"/>
+      <c r="O48" s="69"/>
+      <c r="P48" s="69"/>
+      <c r="Q48" s="69"/>
+      <c r="R48" s="69"/>
+      <c r="S48" s="69"/>
+      <c r="T48" s="69"/>
+      <c r="U48" s="69"/>
+      <c r="V48" s="69"/>
+      <c r="W48" s="69"/>
+      <c r="X48" s="69"/>
+      <c r="Y48" s="69"/>
+      <c r="Z48" s="69"/>
+      <c r="AA48" s="69"/>
+      <c r="AB48" s="69"/>
+      <c r="AC48" s="69"/>
+      <c r="AD48" s="69"/>
+      <c r="AE48" s="69"/>
+      <c r="AF48" s="69"/>
+      <c r="AG48" s="69"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="23.25" outlineLevel="0" r="49">
-      <c r="A49" s="71"/>
-      <c r="B49" s="71"/>
-      <c r="C49" s="71"/>
-      <c r="D49" s="71"/>
-      <c r="E49" s="71"/>
-      <c r="F49" s="71"/>
-      <c r="G49" s="71"/>
-      <c r="H49" s="71"/>
-      <c r="I49" s="71"/>
-      <c r="J49" s="71"/>
-      <c r="K49" s="71"/>
-      <c r="L49" s="71"/>
-      <c r="M49" s="71"/>
-      <c r="N49" s="71"/>
-      <c r="O49" s="71"/>
-      <c r="P49" s="71"/>
-      <c r="Q49" s="71"/>
-      <c r="R49" s="71"/>
-      <c r="S49" s="71"/>
-      <c r="T49" s="71"/>
-      <c r="U49" s="71"/>
-      <c r="V49" s="71"/>
-      <c r="W49" s="71"/>
-      <c r="X49" s="71"/>
-      <c r="Y49" s="71"/>
-      <c r="Z49" s="71"/>
-      <c r="AA49" s="71"/>
-      <c r="AB49" s="71"/>
-      <c r="AC49" s="71"/>
-      <c r="AD49" s="71"/>
-      <c r="AE49" s="71"/>
-      <c r="AF49" s="71"/>
-      <c r="AG49" s="71"/>
+      <c r="A49" s="69"/>
+      <c r="B49" s="69"/>
+      <c r="C49" s="69"/>
+      <c r="D49" s="69"/>
+      <c r="E49" s="69"/>
+      <c r="F49" s="69"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="69"/>
+      <c r="I49" s="69"/>
+      <c r="J49" s="69"/>
+      <c r="K49" s="69"/>
+      <c r="L49" s="69"/>
+      <c r="M49" s="69"/>
+      <c r="N49" s="69"/>
+      <c r="O49" s="69"/>
+      <c r="P49" s="69"/>
+      <c r="Q49" s="69"/>
+      <c r="R49" s="69"/>
+      <c r="S49" s="69"/>
+      <c r="T49" s="69"/>
+      <c r="U49" s="69"/>
+      <c r="V49" s="69"/>
+      <c r="W49" s="69"/>
+      <c r="X49" s="69"/>
+      <c r="Y49" s="69"/>
+      <c r="Z49" s="69"/>
+      <c r="AA49" s="69"/>
+      <c r="AB49" s="69"/>
+      <c r="AC49" s="69"/>
+      <c r="AD49" s="69"/>
+      <c r="AE49" s="69"/>
+      <c r="AF49" s="69"/>
+      <c r="AG49" s="69"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="50">
-      <c r="A50" s="71"/>
-      <c r="B50" s="71"/>
-      <c r="C50" s="71"/>
-      <c r="D50" s="71"/>
-      <c r="E50" s="71"/>
-      <c r="F50" s="71"/>
-      <c r="G50" s="71"/>
-      <c r="H50" s="71"/>
-      <c r="I50" s="71"/>
-      <c r="J50" s="71"/>
-      <c r="K50" s="71"/>
-      <c r="L50" s="71"/>
-      <c r="M50" s="71"/>
-      <c r="N50" s="71"/>
-      <c r="O50" s="71"/>
-      <c r="P50" s="71"/>
-      <c r="Q50" s="71"/>
-      <c r="R50" s="71"/>
-      <c r="S50" s="71"/>
-      <c r="T50" s="71"/>
-      <c r="U50" s="71"/>
-      <c r="V50" s="71"/>
-      <c r="W50" s="71"/>
-      <c r="X50" s="71"/>
-      <c r="Y50" s="71"/>
-      <c r="Z50" s="71"/>
-      <c r="AA50" s="71"/>
-      <c r="AB50" s="71"/>
-      <c r="AC50" s="71"/>
-      <c r="AD50" s="71"/>
-      <c r="AE50" s="71"/>
-      <c r="AF50" s="71"/>
-      <c r="AG50" s="71"/>
+      <c r="A50" s="69"/>
+      <c r="B50" s="69"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="69"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="69"/>
+      <c r="I50" s="69"/>
+      <c r="J50" s="69"/>
+      <c r="K50" s="69"/>
+      <c r="L50" s="69"/>
+      <c r="M50" s="69"/>
+      <c r="N50" s="69"/>
+      <c r="O50" s="69"/>
+      <c r="P50" s="69"/>
+      <c r="Q50" s="69"/>
+      <c r="R50" s="69"/>
+      <c r="S50" s="69"/>
+      <c r="T50" s="69"/>
+      <c r="U50" s="69"/>
+      <c r="V50" s="69"/>
+      <c r="W50" s="69"/>
+      <c r="X50" s="69"/>
+      <c r="Y50" s="69"/>
+      <c r="Z50" s="69"/>
+      <c r="AA50" s="69"/>
+      <c r="AB50" s="69"/>
+      <c r="AC50" s="69"/>
+      <c r="AD50" s="69"/>
+      <c r="AE50" s="69"/>
+      <c r="AF50" s="69"/>
+      <c r="AG50" s="69"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.75" outlineLevel="0" r="51">
-      <c r="A51" s="72" t="s">
+      <c r="A51" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="B51" s="72"/>
-      <c r="C51" s="72"/>
-      <c r="D51" s="72"/>
-      <c r="E51" s="72"/>
-      <c r="F51" s="72"/>
-      <c r="G51" s="72"/>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="72"/>
-      <c r="K51" s="72"/>
-      <c r="L51" s="72"/>
-      <c r="M51" s="72"/>
-      <c r="N51" s="72"/>
-      <c r="O51" s="72"/>
-      <c r="P51" s="72"/>
-      <c r="Q51" s="72"/>
-      <c r="R51" s="72"/>
-      <c r="S51" s="72"/>
-      <c r="T51" s="72"/>
-      <c r="U51" s="72"/>
-      <c r="V51" s="72"/>
-      <c r="W51" s="72"/>
-      <c r="X51" s="72"/>
-      <c r="Y51" s="72"/>
-      <c r="Z51" s="72"/>
-      <c r="AA51" s="72"/>
-      <c r="AB51" s="72"/>
-      <c r="AC51" s="72"/>
-      <c r="AD51" s="72"/>
-      <c r="AE51" s="72"/>
-      <c r="AF51" s="72"/>
-      <c r="AG51" s="72"/>
+      <c r="B51" s="70"/>
+      <c r="C51" s="70"/>
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
+      <c r="J51" s="70"/>
+      <c r="K51" s="70"/>
+      <c r="L51" s="70"/>
+      <c r="M51" s="70"/>
+      <c r="N51" s="70"/>
+      <c r="O51" s="70"/>
+      <c r="P51" s="70"/>
+      <c r="Q51" s="70"/>
+      <c r="R51" s="70"/>
+      <c r="S51" s="70"/>
+      <c r="T51" s="70"/>
+      <c r="U51" s="70"/>
+      <c r="V51" s="70"/>
+      <c r="W51" s="70"/>
+      <c r="X51" s="70"/>
+      <c r="Y51" s="70"/>
+      <c r="Z51" s="70"/>
+      <c r="AA51" s="70"/>
+      <c r="AB51" s="70"/>
+      <c r="AC51" s="70"/>
+      <c r="AD51" s="70"/>
+      <c r="AE51" s="70"/>
+      <c r="AF51" s="70"/>
+      <c r="AG51" s="70"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="10.5" outlineLevel="0" r="52"/>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="53">
-      <c r="A53" s="73" t="s">
+      <c r="A53" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="73"/>
-      <c r="C53" s="73"/>
-      <c r="D53" s="73"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="73"/>
-      <c r="G53" s="73"/>
-      <c r="H53" s="73"/>
-      <c r="I53" s="73"/>
-      <c r="J53" s="73"/>
-      <c r="K53" s="73"/>
-      <c r="L53" s="73"/>
-      <c r="M53" s="73"/>
-      <c r="N53" s="73"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="71"/>
+      <c r="H53" s="71"/>
+      <c r="I53" s="71"/>
+      <c r="J53" s="71"/>
+      <c r="K53" s="71"/>
+      <c r="L53" s="71"/>
+      <c r="M53" s="71"/>
+      <c r="N53" s="71"/>
       <c r="S53" s="27" t="s">
         <v>50</v>
       </c>
@@ -2816,40 +2808,40 @@
       <c r="AG54" s="40"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="8.25" outlineLevel="0" r="55">
-      <c r="A55" s="74" t="s">
+      <c r="A55" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="74"/>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
-      <c r="G55" s="74"/>
-      <c r="H55" s="74"/>
-      <c r="I55" s="74"/>
-      <c r="J55" s="74"/>
-      <c r="K55" s="74"/>
-      <c r="L55" s="74"/>
-      <c r="M55" s="74"/>
-      <c r="N55" s="74"/>
-      <c r="R55" s="68"/>
-      <c r="S55" s="74" t="s">
+      <c r="B55" s="72"/>
+      <c r="C55" s="72"/>
+      <c r="D55" s="72"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="72"/>
+      <c r="G55" s="72"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="72"/>
+      <c r="J55" s="72"/>
+      <c r="K55" s="72"/>
+      <c r="L55" s="72"/>
+      <c r="M55" s="72"/>
+      <c r="N55" s="72"/>
+      <c r="R55" s="66"/>
+      <c r="S55" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="T55" s="74"/>
-      <c r="U55" s="74"/>
-      <c r="V55" s="74"/>
-      <c r="W55" s="74"/>
-      <c r="X55" s="74"/>
-      <c r="Y55" s="74"/>
-      <c r="Z55" s="74"/>
-      <c r="AA55" s="74"/>
-      <c r="AB55" s="74"/>
-      <c r="AC55" s="74"/>
-      <c r="AD55" s="74"/>
-      <c r="AE55" s="74"/>
-      <c r="AF55" s="74"/>
-      <c r="AG55" s="74"/>
+      <c r="T55" s="72"/>
+      <c r="U55" s="72"/>
+      <c r="V55" s="72"/>
+      <c r="W55" s="72"/>
+      <c r="X55" s="72"/>
+      <c r="Y55" s="72"/>
+      <c r="Z55" s="72"/>
+      <c r="AA55" s="72"/>
+      <c r="AB55" s="72"/>
+      <c r="AC55" s="72"/>
+      <c r="AD55" s="72"/>
+      <c r="AE55" s="72"/>
+      <c r="AF55" s="72"/>
+      <c r="AG55" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="142">
@@ -3035,97 +3027,97 @@
       <c r="A1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="73" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="73"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
       <c r="E2" s="24" t="n">
         <v>1950</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
       <c r="E3" s="24" t="n">
         <v>450</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
       <c r="E4" s="24" t="n">
         <v>2500</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3158,58 +3150,58 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="24" outlineLevel="0" r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="81" t="n">
+      <c r="B2" s="79" t="n">
         <v>0.05</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="81" t="n">
+      <c r="B3" s="79" t="n">
         <v>0.07</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="81" t="n">
+      <c r="B4" s="79" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="81" t="n">
+      <c r="B5" s="79" t="n">
         <v>0.12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="81" t="n">
+      <c r="B6" s="79" t="n">
         <v>0.15</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="82" t="s">
+      <c r="B7" s="80" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>